<commit_message>
Added relationship trees excel  report
</commit_message>
<xml_diff>
--- a/Tags&Requirements.xlsx
+++ b/Tags&Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willi\Desktop\CS481\TARGEST.MAC.Final-1.2-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{089A3913-2395-4337-836F-6B124F069F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2C1FA70-0E4F-493B-9806-6BCDE92FB9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="735" windowWidth="19185" windowHeight="10065" xr2:uid="{F0DA605C-2863-410F-B618-8A67C43AE2D5}"/>
+    <workbookView xWindow="15" yWindow="735" windowWidth="19185" windowHeight="10065" xr2:uid="{E5BEF936-2358-4DF6-B43E-2D25EC0C9EED}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -1495,7 +1495,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64C5F73B-9DFC-4195-B4F4-A8E589A825BC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD4A842D-29A0-469A-B5B7-3D97AC2E56A9}">
   <dimension ref="A1:N122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
commented out some print statements
</commit_message>
<xml_diff>
--- a/Tags&Requirements.xlsx
+++ b/Tags&Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willi\Desktop\CS481\TARGEST.MAC.Final-1.2-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2C1FA70-0E4F-493B-9806-6BCDE92FB9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{00B1B742-9061-45A2-98DD-9A528F9E0B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="735" windowWidth="19185" windowHeight="10065" xr2:uid="{E5BEF936-2358-4DF6-B43E-2D25EC0C9EED}"/>
+    <workbookView xWindow="15" yWindow="735" windowWidth="19185" windowHeight="10065" xr2:uid="{CFEDF4F7-7B85-486E-9FDC-E509C2DC9728}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -1495,7 +1495,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD4A842D-29A0-469A-B5B7-3D97AC2E56A9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8460D8B8-B9D3-415C-BC56-258A61525907}">
   <dimension ref="A1:N122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
commented out line 108
push commit
</commit_message>
<xml_diff>
--- a/Tags&Requirements.xlsx
+++ b/Tags&Requirements.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willi\Desktop\CS481\TARGEST.MAC.Final-1.2-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrian/Documents/TARGEST.MAC.Final-1.2-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00B1B742-9061-45A2-98DD-9A528F9E0B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A07C51A4-AFB5-D848-942A-340FD47BC1E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="735" windowWidth="19185" windowHeight="10065" xr2:uid="{CFEDF4F7-7B85-486E-9FDC-E509C2DC9728}"/>
+    <workbookView xWindow="4300" yWindow="2700" windowWidth="27640" windowHeight="16940" xr2:uid="{4724FAE4-607E-F644-9A25-4FEC48076569}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="342">
   <si>
     <t>PUMP:HRD:100</t>
   </si>
@@ -68,9 +68,6 @@
     <t xml:space="preserve">Details regarding the full color touchscreen. </t>
   </si>
   <si>
-    <t>PUMP:HRD:0000</t>
-  </si>
-  <si>
     <t>PUMP:HRS:100</t>
   </si>
   <si>
@@ -116,25 +113,25 @@
     <t>PUMP:HTP:200</t>
   </si>
   <si>
-    <t xml:space="preserve">HTP:200 Test 200 </t>
+    <t xml:space="preserve">Test 200 </t>
   </si>
   <si>
     <t>PUMP:HTP:300</t>
   </si>
   <si>
-    <t xml:space="preserve">HTP:300 Test 300 </t>
+    <t xml:space="preserve">Test 300 </t>
   </si>
   <si>
     <t>PUMP:HTP:400</t>
   </si>
   <si>
-    <t xml:space="preserve">HTP:400 Test 400 </t>
+    <t xml:space="preserve">Test 400 </t>
   </si>
   <si>
     <t>PUMP:HTP:500</t>
   </si>
   <si>
-    <t xml:space="preserve">HTP:500 Test 500 </t>
+    <t xml:space="preserve">Test 500 </t>
   </si>
   <si>
     <t>PUMP:HTP:1100</t>
@@ -170,60 +167,33 @@
     <t>PUMP:HTR:100</t>
   </si>
   <si>
-    <t>PUMPHTR:200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HTR:200 Test 200 </t>
+    <t>PUMP:HTR:200</t>
   </si>
   <si>
     <t>PUMP:HTR:300</t>
   </si>
   <si>
-    <t xml:space="preserve">HTR:300 Test 300 </t>
-  </si>
-  <si>
     <t>PUMP:HTR:400</t>
   </si>
   <si>
-    <t xml:space="preserve">HTR:400 Test 400 </t>
-  </si>
-  <si>
     <t>PUMP:HTR:500</t>
   </si>
   <si>
-    <t xml:space="preserve">HTR:500 Test 500 </t>
-  </si>
-  <si>
     <t>PUMP:HTR:1100</t>
   </si>
   <si>
-    <t xml:space="preserve">HTR:1100 Test 1100 </t>
-  </si>
-  <si>
     <t>PUMP:HTR:1200</t>
   </si>
   <si>
-    <t xml:space="preserve">HTR:1200 Test 1200 </t>
-  </si>
-  <si>
     <t>PUMP:HTR:1300</t>
   </si>
   <si>
-    <t xml:space="preserve">HTR:1300 Test 1300 </t>
-  </si>
-  <si>
     <t>PUMP:HTR:1400</t>
   </si>
   <si>
-    <t xml:space="preserve">HTR:1400 Test 1400 </t>
-  </si>
-  <si>
     <t>PUMP:HTR:1500</t>
   </si>
   <si>
-    <t xml:space="preserve">HTR:1500 Test 1500 </t>
-  </si>
-  <si>
     <t>PUMP:PRS:1</t>
   </si>
   <si>
@@ -413,7 +383,7 @@
     <t>BOLUS:SRS:2</t>
   </si>
   <si>
-    <t xml:space="preserve">The bolus size shall be estimated as the sum of the insulin needed to cover the current meal  and correct down to 110 mg/dL. If the sum is negative, the bolus is aborted.  </t>
+    <t xml:space="preserve">The bolus size shall be estimated as the sum of the insulin needed to cover the current meal  and correct down to 110 mg/dL. If the sum is negative, the bolus is aborted. </t>
   </si>
   <si>
     <t>BOLUS:SRS:5</t>
@@ -506,27 +476,15 @@
     <t>PUMP:SVATR:200</t>
   </si>
   <si>
-    <t xml:space="preserve">Test 200 </t>
-  </si>
-  <si>
     <t>PUMP:SVATR:300</t>
   </si>
   <si>
-    <t xml:space="preserve">Test 300 </t>
-  </si>
-  <si>
     <t>PUMP:SVATR:400</t>
   </si>
   <si>
-    <t xml:space="preserve">Test 400 </t>
-  </si>
-  <si>
     <t>PUMP:SVATR:500</t>
   </si>
   <si>
-    <t xml:space="preserve">Test 500 </t>
-  </si>
-  <si>
     <t>PUMP:UT:100</t>
   </si>
   <si>
@@ -785,9 +743,6 @@
     <t>PUMP:HRS:103</t>
   </si>
   <si>
-    <t>PUMP:TBV:1111</t>
-  </si>
-  <si>
     <t>PUMP:PRS:103</t>
   </si>
   <si>
@@ -851,9 +806,6 @@
     <t>PUMP:UNIT:220</t>
   </si>
   <si>
-    <t>[PUMP:TBV:1111]</t>
-  </si>
-  <si>
     <t>[PUMP:TBV:1]</t>
   </si>
   <si>
@@ -878,6 +830,9 @@
     <t>[PUMP:HRS:3330]</t>
   </si>
   <si>
+    <t>[PUMP:HRS:3350]</t>
+  </si>
+  <si>
     <t>[PUMP:PRS:100]</t>
   </si>
   <si>
@@ -896,9 +851,6 @@
     <t>[PUMP:HRS:105]</t>
   </si>
   <si>
-    <t>[PUMP:HRS:3350]</t>
-  </si>
-  <si>
     <t>[PUMP:HRD:100]</t>
   </si>
   <si>
@@ -1019,7 +971,7 @@
     <t>[PUMP:PRS:105]</t>
   </si>
   <si>
-    <t>[PUMP:PRS:1] [PUMP:TBD:1]</t>
+    <t>[PUMP:PRS:1][PUMP:TBD:1]</t>
   </si>
   <si>
     <t>[PUMP:PRS:1] [PUMP:PRS:5]</t>
@@ -1118,7 +1070,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1495,56 +1447,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8460D8B8-B9D3-415C-BC56-258A61525907}">
-  <dimension ref="A1:N122"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB0142FC-3A8A-3348-90ED-9184E9FFBA4E}">
+  <dimension ref="A1:N121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="168.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="102.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.73046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.46484375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.73046875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="1.73046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.06640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="1.73046875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="179.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="111.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1561,34 +1513,34 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1605,28 +1557,22 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1643,22 +1589,22 @@
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="G4">
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="I4">
         <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1675,22 +1621,22 @@
         <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="G5">
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="I5">
         <v>3</v>
       </c>
       <c r="J5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1707,22 +1653,22 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="G6">
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="I6">
         <v>4</v>
       </c>
       <c r="J6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1730,7 +1676,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1739,534 +1685,534 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="G7">
         <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="I7">
         <v>5</v>
       </c>
       <c r="J7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8">
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="G8">
         <v>6</v>
       </c>
       <c r="H8" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="I8">
         <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="G9">
         <v>7</v>
       </c>
       <c r="H9" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="I9">
         <v>7</v>
       </c>
       <c r="J9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10">
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="G10">
         <v>8</v>
       </c>
       <c r="H10" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="I10">
         <v>8</v>
       </c>
       <c r="J10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D11">
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="G11">
         <v>9</v>
       </c>
       <c r="H11" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="I11">
         <v>9</v>
       </c>
       <c r="J11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D12">
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="G12">
         <v>10</v>
       </c>
       <c r="H12" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="I12">
         <v>10</v>
       </c>
       <c r="J12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D13">
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F13" t="s">
-        <v>284</v>
+        <v>260</v>
       </c>
       <c r="G13">
         <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="I13">
         <v>11</v>
       </c>
       <c r="J13" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D14">
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="G14">
         <v>12</v>
       </c>
       <c r="H14" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="I14">
         <v>12</v>
       </c>
       <c r="J14" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D15">
         <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
       <c r="G15">
         <v>13</v>
       </c>
       <c r="H15" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="I15">
         <v>13</v>
       </c>
       <c r="J15" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D16">
         <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F16" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="G16">
         <v>14</v>
       </c>
       <c r="H16" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="I16">
         <v>14</v>
       </c>
       <c r="J16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D17">
         <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F17" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="G17">
         <v>15</v>
       </c>
       <c r="H17" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="I17">
         <v>15</v>
       </c>
       <c r="J17" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D18">
         <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F18" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="G18">
         <v>16</v>
       </c>
       <c r="H18" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="I18">
         <v>16</v>
       </c>
       <c r="J18" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D19">
         <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F19" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="G19">
         <v>17</v>
       </c>
       <c r="H19" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="I19">
         <v>17</v>
       </c>
       <c r="J19" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D20">
         <v>18</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F20" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="G20">
         <v>18</v>
       </c>
       <c r="H20" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="I20">
         <v>18</v>
       </c>
       <c r="J20" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D21">
         <v>19</v>
       </c>
       <c r="E21" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F21" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="G21">
         <v>19</v>
       </c>
       <c r="H21" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="I21">
         <v>19</v>
       </c>
       <c r="J21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F22" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="G22">
         <v>20</v>
       </c>
       <c r="H22" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="I22">
         <v>20</v>
       </c>
       <c r="J22" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D23">
         <v>21</v>
       </c>
       <c r="E23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F23" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="G23">
         <v>21</v>
       </c>
       <c r="H23" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="I23">
         <v>21</v>
       </c>
       <c r="J23" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2274,7 +2220,7 @@
         <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D24">
         <v>22</v>
@@ -2283,22 +2229,22 @@
         <v>43</v>
       </c>
       <c r="F24" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="G24">
         <v>22</v>
       </c>
       <c r="H24" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="I24">
         <v>22</v>
       </c>
       <c r="J24" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2306,7 +2252,7 @@
         <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="D25">
         <v>23</v>
@@ -2315,2166 +2261,2134 @@
         <v>44</v>
       </c>
       <c r="F25" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="G25">
         <v>23</v>
       </c>
       <c r="H25" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="I25">
         <v>23</v>
       </c>
       <c r="J25" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D26">
         <v>24</v>
       </c>
       <c r="E26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F26" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="G26">
         <v>24</v>
       </c>
       <c r="H26" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="I26">
         <v>24</v>
       </c>
       <c r="J26" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="D27">
         <v>25</v>
       </c>
       <c r="E27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F27" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="G27">
         <v>25</v>
       </c>
       <c r="H27" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="I27">
         <v>25</v>
       </c>
       <c r="J27" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="D28">
         <v>26</v>
       </c>
       <c r="E28" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F28" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="G28">
         <v>26</v>
       </c>
       <c r="H28" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="I28">
         <v>26</v>
       </c>
       <c r="J28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="D29">
         <v>27</v>
       </c>
       <c r="E29" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F29" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="G29">
         <v>27</v>
       </c>
       <c r="H29" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="I29">
         <v>27</v>
       </c>
       <c r="J29" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D30">
         <v>28</v>
       </c>
       <c r="E30" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F30" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="G30">
         <v>28</v>
       </c>
       <c r="H30" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="I30">
         <v>28</v>
       </c>
       <c r="J30" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="D31">
         <v>29</v>
       </c>
       <c r="E31" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F31" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="G31">
         <v>29</v>
       </c>
       <c r="H31" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="I31">
         <v>29</v>
       </c>
       <c r="J31" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C32" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D32">
         <v>30</v>
       </c>
       <c r="E32" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F32" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="G32">
         <v>30</v>
       </c>
       <c r="H32" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="I32">
         <v>30</v>
       </c>
       <c r="J32" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D33">
         <v>31</v>
       </c>
       <c r="E33" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F33" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="G33">
         <v>31</v>
       </c>
       <c r="H33" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="I33">
         <v>31</v>
       </c>
       <c r="J33" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D34">
         <v>32</v>
       </c>
       <c r="E34" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F34" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="G34">
         <v>32</v>
       </c>
       <c r="H34" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="I34">
         <v>32</v>
       </c>
       <c r="J34" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C35" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D35">
         <v>33</v>
       </c>
       <c r="E35" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F35" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="G35">
         <v>33</v>
       </c>
       <c r="H35" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="I35">
         <v>33</v>
       </c>
       <c r="J35" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C36" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D36">
         <v>34</v>
       </c>
       <c r="E36" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F36" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="G36">
         <v>34</v>
       </c>
       <c r="H36" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="I36">
         <v>34</v>
       </c>
       <c r="J36" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C37" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D37">
         <v>35</v>
       </c>
       <c r="E37" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="F37" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
       <c r="G37">
         <v>35</v>
       </c>
       <c r="H37" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="I37">
         <v>35</v>
       </c>
       <c r="J37" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C38" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D38">
         <v>36</v>
       </c>
       <c r="E38" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F38" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="G38">
         <v>36</v>
       </c>
       <c r="H38" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="I38">
         <v>36</v>
       </c>
       <c r="J38" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C39" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D39">
         <v>37</v>
       </c>
       <c r="E39" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="F39" t="s">
-        <v>306</v>
-      </c>
-      <c r="G39">
-        <v>37</v>
-      </c>
-      <c r="H39" t="s">
-        <v>270</v>
+        <v>291</v>
       </c>
       <c r="I39">
         <v>37</v>
       </c>
       <c r="J39" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C40" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="D40">
         <v>38</v>
       </c>
       <c r="E40" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="F40" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="I40">
         <v>38</v>
       </c>
       <c r="J40" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C41" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="D41">
         <v>39</v>
       </c>
       <c r="E41" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F41" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="I41">
         <v>39</v>
       </c>
       <c r="J41" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C42" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D42">
         <v>40</v>
       </c>
       <c r="E42" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="F42" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="I42">
         <v>40</v>
       </c>
       <c r="J42" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C43" t="s">
-        <v>80</v>
+        <v>17</v>
       </c>
       <c r="D43">
         <v>41</v>
       </c>
       <c r="E43" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="F43" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="I43">
         <v>41</v>
       </c>
       <c r="J43" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C44" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D44">
         <v>42</v>
       </c>
       <c r="E44" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F44" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="I44">
         <v>42</v>
       </c>
       <c r="J44" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C45" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D45">
         <v>43</v>
       </c>
       <c r="E45" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="F45" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="I45">
         <v>43</v>
       </c>
       <c r="J45" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C46" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="D46">
         <v>44</v>
       </c>
       <c r="E46" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F46" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="I46">
         <v>44</v>
       </c>
       <c r="J46" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C47" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D47">
         <v>45</v>
       </c>
       <c r="E47" t="s">
-        <v>84</v>
-      </c>
-      <c r="F47" t="s">
-        <v>313</v>
+        <v>76</v>
       </c>
       <c r="I47">
         <v>45</v>
       </c>
       <c r="J47" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C48" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D48">
         <v>46</v>
       </c>
       <c r="E48" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="I48">
         <v>46</v>
       </c>
       <c r="J48" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C49" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D49">
         <v>47</v>
       </c>
       <c r="E49" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="I49">
         <v>47</v>
       </c>
       <c r="J49" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C50" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D50">
         <v>48</v>
       </c>
       <c r="E50" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="I50">
         <v>48</v>
       </c>
       <c r="J50" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C51" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D51">
         <v>49</v>
       </c>
       <c r="E51" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="I51">
         <v>49</v>
       </c>
       <c r="J51" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C52" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D52">
         <v>50</v>
       </c>
       <c r="E52" t="s">
-        <v>94</v>
+        <v>86</v>
+      </c>
+      <c r="F52" t="s">
+        <v>298</v>
       </c>
       <c r="I52">
         <v>50</v>
       </c>
       <c r="J52" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C53" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D53">
         <v>51</v>
       </c>
       <c r="E53" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F53" t="s">
-        <v>314</v>
-      </c>
-      <c r="I53">
-        <v>51</v>
-      </c>
-      <c r="J53" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C54" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D54">
         <v>52</v>
       </c>
       <c r="E54" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F54" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C55" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D55">
         <v>53</v>
       </c>
       <c r="E55" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F55" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C56" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D56">
         <v>54</v>
       </c>
       <c r="E56" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F56" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C57" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D57">
         <v>55</v>
       </c>
       <c r="E57" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="F57" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C58" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D58">
         <v>56</v>
       </c>
       <c r="E58" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F58" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C59" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D59">
         <v>57</v>
       </c>
       <c r="E59" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F59" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C60" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D60">
         <v>58</v>
       </c>
       <c r="E60" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F60" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C61" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D61">
         <v>59</v>
       </c>
       <c r="E61" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="F61" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C62" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D62">
         <v>60</v>
       </c>
       <c r="E62" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="F62" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C63" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D63">
         <v>61</v>
       </c>
       <c r="E63" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F63" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C64" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D64">
         <v>62</v>
       </c>
       <c r="E64" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="F64" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C65" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D65">
         <v>63</v>
       </c>
       <c r="E65" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="F65" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C66" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D66">
         <v>64</v>
       </c>
       <c r="E66" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F66" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C67" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D67">
         <v>65</v>
       </c>
       <c r="E67" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F67" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C68" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="D68">
         <v>66</v>
       </c>
       <c r="E68" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F68" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C69" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D69">
         <v>67</v>
       </c>
       <c r="E69" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="F69" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C70" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D70">
         <v>68</v>
       </c>
       <c r="E70" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F70" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C71" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D71">
         <v>69</v>
       </c>
       <c r="E71" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="F71" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C72" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D72">
         <v>70</v>
       </c>
       <c r="E72" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="F72" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C73" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D73">
         <v>71</v>
       </c>
       <c r="E73" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="F73" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C74" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D74">
         <v>72</v>
       </c>
       <c r="E74" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="F74" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C75" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D75">
         <v>73</v>
       </c>
       <c r="E75" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="F75" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C76" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D76">
         <v>74</v>
       </c>
       <c r="E76" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="F76" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C77" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D77">
         <v>75</v>
       </c>
       <c r="E77" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="F77" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C78" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D78">
         <v>76</v>
       </c>
       <c r="E78" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F78" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C79" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D79">
         <v>77</v>
       </c>
       <c r="E79" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="F79" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C80" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D80">
         <v>78</v>
       </c>
       <c r="E80" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="F80" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C81" t="s">
-        <v>153</v>
+        <v>23</v>
       </c>
       <c r="D81">
         <v>79</v>
       </c>
       <c r="E81" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="F81" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C82" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D82">
         <v>80</v>
       </c>
       <c r="E82" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="F82" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C83" t="s">
-        <v>156</v>
+        <v>27</v>
       </c>
       <c r="D83">
         <v>81</v>
       </c>
       <c r="E83" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="F83" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C84" t="s">
-        <v>158</v>
+        <v>29</v>
       </c>
       <c r="D84">
         <v>82</v>
       </c>
       <c r="E84" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="F84" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="C85" t="s">
-        <v>160</v>
+        <v>31</v>
       </c>
       <c r="D85">
         <v>83</v>
       </c>
       <c r="E85" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="F85" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="C86" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="D86">
         <v>84</v>
       </c>
       <c r="E86" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="F86" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="C87" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="D87">
         <v>85</v>
       </c>
       <c r="E87" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="F87" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C88" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="D88">
         <v>86</v>
       </c>
       <c r="E88" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="F88" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="C89" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="D89">
         <v>87</v>
       </c>
       <c r="E89" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="F89" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="C90" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="D90">
         <v>88</v>
       </c>
       <c r="E90" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="F90" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="C91" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="D91">
         <v>89</v>
       </c>
       <c r="E91" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="F91" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="C92" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="D92">
         <v>90</v>
       </c>
       <c r="E92" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="F92" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="C93" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="D93">
         <v>91</v>
       </c>
       <c r="E93" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="F93" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="C94" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="D94">
         <v>92</v>
       </c>
       <c r="E94" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="F94" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="C95" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="D95">
         <v>93</v>
       </c>
       <c r="E95" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="F95" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="C96" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="D96">
         <v>94</v>
       </c>
       <c r="E96" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="F96" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="C97" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="D97">
         <v>95</v>
       </c>
       <c r="E97" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="F97" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="C98" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="D98">
         <v>96</v>
       </c>
       <c r="E98" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="F98" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="C99" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="D99">
         <v>97</v>
       </c>
       <c r="E99" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="F99" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="C100" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="D100">
         <v>98</v>
       </c>
       <c r="E100" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="F100" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="C101" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="D101">
         <v>99</v>
       </c>
       <c r="E101" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="F101" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="C102" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="D102">
         <v>100</v>
       </c>
       <c r="E102" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="F102" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="C103" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="D103">
         <v>101</v>
       </c>
       <c r="E103" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="F103" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="C104" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="D104">
         <v>102</v>
       </c>
       <c r="E104" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="F104" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="C105" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="D105">
         <v>103</v>
       </c>
       <c r="E105" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="F105" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="C106" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="D106">
         <v>104</v>
       </c>
       <c r="E106" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="F106" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="C107" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="D107">
         <v>105</v>
       </c>
       <c r="E107" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="F107" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="C108" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="D108">
         <v>106</v>
       </c>
       <c r="E108" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="F108" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="C109" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="D109">
         <v>107</v>
       </c>
       <c r="E109" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="F109" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="C110" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="D110">
         <v>108</v>
       </c>
       <c r="E110" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="F110" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="C111" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="D111">
         <v>109</v>
       </c>
       <c r="E111" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="F111" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="C112" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="D112">
         <v>110</v>
       </c>
       <c r="E112" t="s">
-        <v>213</v>
-      </c>
-      <c r="F112" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.45">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="C113" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="D113">
         <v>111</v>
       </c>
       <c r="E113" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.45">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="C114" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="D114">
         <v>112</v>
       </c>
       <c r="E114" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.45">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="C115" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="D115">
         <v>113</v>
       </c>
       <c r="E115" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.45">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="C116" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="D116">
         <v>114</v>
       </c>
       <c r="E116" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.45">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="C117" t="s">
-        <v>224</v>
+        <v>83</v>
       </c>
       <c r="D117">
         <v>115</v>
       </c>
       <c r="E117" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.45">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="C118" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D118">
         <v>116</v>
       </c>
       <c r="E118" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.45">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="C119" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
       <c r="D119">
         <v>117</v>
       </c>
       <c r="E119" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.45">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="C120" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="D120">
         <v>118</v>
       </c>
       <c r="E120" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.45">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="C121" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="D121">
         <v>119</v>
       </c>
       <c r="E121" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A122">
-        <v>120</v>
-      </c>
-      <c r="B122" t="s">
-        <v>231</v>
-      </c>
-      <c r="C122" t="s">
-        <v>232</v>
-      </c>
-      <c r="D122">
-        <v>120</v>
-      </c>
-      <c r="E122" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>